<commit_message>
update script create tb dim fact
</commit_message>
<xml_diff>
--- a/Dim_Fact/star schema.xlsx
+++ b/Dim_Fact/star schema.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Do an Cuoi Khoa - 30.5.23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Do an Cuoi Khoa - 30.5.23\Tai lieu do an full\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470694DE-8A4F-4AB8-814E-3611BB95DB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0244B500-6437-4AC7-8F52-80F27F24A8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EDD0DD81-E8CC-4B8B-BD10-CC2BE3427AE3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="NOW" sheetId="1" r:id="rId1"/>
+    <sheet name="Old" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>order_date</t>
   </si>
@@ -49,6 +50,12 @@
   </si>
   <si>
     <t>lấy từ bảng order_details</t>
+  </si>
+  <si>
+    <t>Cước phí vận chuyển</t>
+  </si>
+  <si>
+    <t>Customer Sales = unit_price*quantity*discount</t>
   </si>
 </sst>
 </file>
@@ -125,13 +132,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1569854</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>137433</xdr:rowOff>
@@ -258,15 +265,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>8964</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>47065</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:colOff>1190064</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>266</xdr:rowOff>
+      <xdr:rowOff>9231</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -289,8 +296,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3459480" y="784860"/>
-          <a:ext cx="1181100" cy="3071126"/>
+          <a:off x="3469340" y="782171"/>
+          <a:ext cx="1181100" cy="3010166"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -301,13 +308,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1264920</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
@@ -352,23 +359,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1607820</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>80682</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1231402</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>160117</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46CD4722-A52E-1D93-AB1A-45DE3AAAE6A4}"/>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6CC60A5-5AB3-8851-0FFC-4D12F47CA28C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -384,6 +391,924 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
+          <a:off x="6248400" y="4473389"/>
+          <a:ext cx="1150720" cy="1083480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>69924</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>43478</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1226472</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>8992</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D681A1FE-C03A-0D98-289D-315499F71C67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6237642" y="5619525"/>
+          <a:ext cx="1156548" cy="324103"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104888</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>130437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1019367</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>157365</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{485A682A-239B-E68B-CB44-99B132A8793D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6272606" y="6065072"/>
+          <a:ext cx="914479" cy="385516"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>174364</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1134932</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>174364</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2147193F-CE37-4D00-A803-0B164C673305}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2075330" y="1268058"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>40341</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>75752</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1152861</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>75752</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BCE67F5-2BAE-48C3-A617-C1E692834467}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2093259" y="1528034"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>121023</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>120575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1233543</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>120575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{870F21D7-D301-407B-8510-01A20C0035F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6288741" y="2110740"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>766482</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>107576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2572870</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>156434</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55FC81EC-3784-4CFA-9410-34D5336103FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6934200" y="2277035"/>
+          <a:ext cx="1806388" cy="48858"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>156882</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12998</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1269402</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12998</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3B95D09-274D-46D9-924C-493F62620601}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6324600" y="2541045"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>165847</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66787</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1278367</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66787</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F46941DF-E1FC-4DDD-8434-912CF02FF78C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6333565" y="2774128"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>174811</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>93682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1287331</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>93682</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC19E07-5967-469B-96FA-1B0432A8090D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6342529" y="2980317"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85164</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>147470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1197684</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>147470</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76BBA3D7-3C6A-43C6-BEE2-55EF97174279}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6252882" y="3213399"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>165846</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>21964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1278366</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>21964</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89C9A8B7-A730-4308-ACAC-54E12F49D202}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6333564" y="3446482"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219635</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66788</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1332155</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66788</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B49BBE3-9555-4137-A782-F89CEE0D7FF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6387353" y="3670600"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>143434</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161363</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1035051</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152908</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36FF0B33-5DDF-83B8-C1C1-9CF76C49592F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6311152" y="3765175"/>
+          <a:ext cx="891617" cy="708721"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1569854</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>137433</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AE8185B-878D-4CBB-A0CB-A9CA7C27DD47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6195060" y="662940"/>
+          <a:ext cx="1546994" cy="3147333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1272650</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>23076</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8354141-B052-4822-A9AF-6FC39399C5FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="655320"/>
+          <a:ext cx="1272650" cy="2491956"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1424940</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1264920</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1643FEC1-4A1C-4B5A-9937-DB72F6C9F62F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2034540" y="579120"/>
+          <a:ext cx="1280160" cy="2567940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>266</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{170E422F-395B-408B-8D0A-1F01335210C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3459480" y="784860"/>
+          <a:ext cx="1181100" cy="3071126"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1264920</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8026A397-0BF9-4419-B401-731081E74CD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6324600" y="1196340"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1607820</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FC26B3D-8C60-4A00-A2FA-DB0B0230A5EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
           <a:off x="6172200" y="3855720"/>
           <a:ext cx="1607820" cy="1082040"/>
         </a:xfrm>
@@ -409,10 +1334,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Right Brace 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29DF854A-EA35-6589-17F0-40E2D22EA402}"/>
+        <xdr:cNvPr id="8" name="Right Brace 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C4E30E5-FB3F-4D86-8BCE-CB7E38A86B12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -467,10 +1392,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6CC60A5-5AB3-8851-0FFC-4D12F47CA28C}"/>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{825B8170-3F87-48D9-A223-887B0178EA4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -511,10 +1436,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D681A1FE-C03A-0D98-289D-315499F71C67}"/>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F32EC780-E0E8-43B1-91DF-EA6A04F74A20}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -555,10 +1480,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{485A682A-239B-E68B-CB44-99B132A8793D}"/>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96F214AA-3581-4EBD-9607-FD88BB8C921F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -582,6 +1507,108 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>174364</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1134932</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>174364</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F92FC7E-5178-4785-BA27-7D7D1E45CCF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2072192" y="1286884"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>40341</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>75752</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1152861</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>75752</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA488141-5588-4655-B50E-9282EBF6E9E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2090121" y="1554032"/>
+          <a:ext cx="1112520" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -884,10 +1911,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FADBADB-E69F-4997-B02D-252E0D2C0AB9}">
+  <dimension ref="B3:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="37.77734375" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCC8911-7562-45F7-917B-7ED00309D103}">
   <dimension ref="B3:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>